<commit_message>
Updated PoiFormulaHelper to use newly added utility methods - Updated tests
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/PoiFormulaHelperTest.xlsx
+++ b/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/PoiFormulaHelperTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanco/ws-epsilon/emc-cellsheet/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D60B567-719D-4F45-BB5B-0189BAF77712}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05423C1D-D3AB-224D-8E83-F95006F9B613}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-76800" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
   </bookViews>
   <sheets>
     <sheet name="PoiFormulaHelperTest" sheetId="1" r:id="rId1"/>
@@ -376,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4252C82E-34D7-43AB-88EB-EAE289BCD8A4}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -397,6 +397,18 @@
       <c r="A2">
         <f>SUM(Data!B1,Data!D5,Data!B5,Data!D2,Data!C2)</f>
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>(6*12)+2</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>6*(12+2)</f>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added utility method for building Formula Strings from Trees
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/PoiFormulaHelperTest.xlsx
+++ b/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/PoiFormulaHelperTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanco/ws-epsilon/emc-cellsheet/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05423C1D-D3AB-224D-8E83-F95006F9B613}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F22446-E476-6349-9ADE-3F2C42D4471D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
+    <workbookView xWindow="-76800" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
   </bookViews>
   <sheets>
     <sheet name="PoiFormulaHelperTest" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Arithmetic no brackets</t>
+  </si>
+  <si>
+    <t>Arithmetic 1 bracket</t>
+  </si>
+  <si>
+    <t>Arithmetic 1 bracket variation</t>
+  </si>
+  <si>
+    <t>Aritmetic 2 sets of brackets</t>
+  </si>
+  <si>
+    <t>SUM over 1 operand or</t>
+  </si>
+  <si>
+    <t>SUM over multiple operands</t>
+  </si>
+  <si>
+    <t>Unary operation formula</t>
+  </si>
+  <si>
+    <t>Percentage formula</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4252C82E-34D7-43AB-88EB-EAE289BCD8A4}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -387,28 +412,76 @@
     <col min="1" max="1" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <f>SUM(Data!A1:D5)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SUM(Data!B1,Data!D5,Data!B5,Data!D2,Data!C2)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f>(6*12)+2</f>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <f>65+20</f>
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f>6*(12+2)</f>
-        <v>84</v>
+        <f>(6*5)+500</f>
+        <v>530</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f>6*(5+500)</f>
+        <v>3030</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f>(34*45)+(235/65)</f>
+        <v>1533.6153846153845</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f>-(8-4)</f>
+        <v>-4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f>9%</f>
+        <v>0.09</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added formula string evaluation - Added helper function in PoiFormulaHelper to handle arbitrary formula string evaluation - Implemented evaluate in ExcelFormulaTree - Modified tests to check evaluation of built formula string
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/PoiFormulaHelperTest.xlsx
+++ b/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/PoiFormulaHelperTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanco/ws-epsilon/emc-cellsheet/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F22446-E476-6349-9ADE-3F2C42D4471D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFD05E2-4329-2C4B-9A9C-6E93B4B031A8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-76800" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
   </bookViews>
@@ -404,7 +404,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -459,8 +459,8 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f>(34*45)+(235/65)</f>
-        <v>1533.6153846153845</v>
+        <f>(34*45)+(800/40)</f>
+        <v>1550</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Renamed variable names for concisness. - Added missing files
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/PoiFormulaHelperTest.xlsx
+++ b/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/PoiFormulaHelperTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanco/ws-epsilon/emc-cellsheet/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFD05E2-4329-2C4B-9A9C-6E93B4B031A8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D88FBD3-7194-1B40-AF19-B324CD15E1D2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-76800" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Arithmetic no brackets</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Percentage formula</t>
+  </si>
+  <si>
+    <t>Multiple Function Eval</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4252C82E-34D7-43AB-88EB-EAE289BCD8A4}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -484,6 +487,15 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f>SUM(Data!A1:D5)+SUM(Data!A1:D5)</f>
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -494,7 +506,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added unit test for partial tree evaluation
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/PoiFormulaHelperTest.xlsx
+++ b/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/PoiFormulaHelperTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanco/ws-epsilon/emc-cellsheet/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D88FBD3-7194-1B40-AF19-B324CD15E1D2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAE50DE-5949-1A4B-91A4-82316347DE06}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-76800" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -489,8 +489,8 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f>SUM(Data!A1:D5)+SUM(Data!A1:D5)</f>
-        <v>40</v>
+        <f>SUM(Data!A1:D5)+SUM(Data!B1:D5)</f>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>

</xml_diff>